<commit_message>
add testing for complex numbers
</commit_message>
<xml_diff>
--- a/factorielTest/factorialClassTestExcel.xlsx
+++ b/factorielTest/factorialClassTestExcel.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t>FactorielClassTest/testFactorielCell(cell=value3)</t>
+  </si>
+  <si>
+    <t>FactorielClassTest/testComplexNumbers(complexNumbers=value1)</t>
+  </si>
+  <si>
+    <t>FactorielClassTest/testComplexNumbers(complexNumbers=value2)</t>
+  </si>
+  <si>
+    <t>FactorielClassTest/testComplexNumbers(complexNumbers=value3)</t>
   </si>
 </sst>
 </file>
@@ -428,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -476,7 +485,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>4.5131600000000001E-2</v>
+        <v>4.49395E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -493,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>3.7330000000000002E-3</v>
+        <v>2.7536000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -510,7 +519,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2.2312E-3</v>
+        <v>2.2372999999999998E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -527,7 +536,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>2.5292000000000001E-3</v>
+        <v>2.6535E-3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -544,7 +553,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>2.3674999999999998E-3</v>
+        <v>2.2807000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -561,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>6.2462000000000004E-3</v>
+        <v>7.8133999999999999E-3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -578,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>5.4710999999999996E-3</v>
+        <v>4.5890999999999996E-3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -595,7 +604,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>5.6873999999999996E-3</v>
+        <v>4.4361000000000001E-3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -612,7 +621,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>5.6020999999999996E-3</v>
+        <v>3.7888000000000002E-3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -629,7 +638,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>5.4132E-3</v>
+        <v>6.0623999999999999E-3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -646,7 +655,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>5.1675999999999996E-3</v>
+        <v>4.2094000000000003E-3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -663,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>6.6084000000000004E-3</v>
+        <v>4.9696000000000002E-3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -680,7 +689,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>5.8798000000000001E-3</v>
+        <v>5.6153000000000002E-3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -697,7 +706,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>5.7857000000000004E-3</v>
+        <v>4.4783999999999996E-3</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -714,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>4.9569999999999996E-3</v>
+        <v>4.7476999999999997E-3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -731,7 +740,7 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>8.2260000000000007E-3</v>
+        <v>3.7507999999999999E-3</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -748,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>6.3623000000000004E-3</v>
+        <v>4.7330000000000002E-3</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -765,7 +774,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>3.9576000000000004E-3</v>
+        <v>4.6677999999999997E-3</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -782,7 +791,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>4.4996000000000003E-3</v>
+        <v>4.8193000000000003E-3</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -799,7 +808,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>6.3708000000000002E-3</v>
+        <v>5.6896000000000004E-3</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -816,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>6.6362000000000001E-3</v>
+        <v>5.1992000000000002E-3</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -833,7 +842,58 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>3.7767700000000001E-2</v>
+        <v>6.6391000000000002E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="b">
+        <v>1</v>
+      </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>4.6625E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="b">
+        <v>1</v>
+      </c>
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>4.0134000000000003E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="b">
+        <v>1</v>
+      </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>3.59294E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>